<commit_message>
Added pickle function to save models
</commit_message>
<xml_diff>
--- a/Decision Matrices/hierarchy.xlsx
+++ b/Decision Matrices/hierarchy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc3adef44a32c2c0/Documents/GitHub/DP4/Decision Matrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1138" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CA594DC-CD4E-4E01-A01C-E452544014E3}"/>
+  <xr:revisionPtr revIDLastSave="1139" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4157974-9CDF-488D-A43E-8FBFDA5B1E6F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5770647-7F3F-411D-B267-99FA93025A86}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>Tier 1</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Model Name:</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
@@ -802,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174D7823-B3F8-4046-8216-CB48ECCFAD7A}">
   <dimension ref="A1:AI117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I100" sqref="I100"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,6 +911,9 @@
       <c r="D2" s="50"/>
       <c r="E2" s="50"/>
       <c r="F2" s="50"/>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
       <c r="H2" s="21" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Added first 3 input checks
</commit_message>
<xml_diff>
--- a/Decision Matrices/hierarchy.xlsx
+++ b/Decision Matrices/hierarchy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc3adef44a32c2c0/Documents/GitHub/DP4/Decision Matrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1164" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D7F3E1A-E5B8-4992-9F39-4BFD89E3FF36}"/>
+  <xr:revisionPtr revIDLastSave="1166" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{783BC90D-2664-4CC3-B68A-4B11ED72BB32}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5770647-7F3F-411D-B267-99FA93025A86}"/>
   </bookViews>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174D7823-B3F8-4046-8216-CB48ECCFAD7A}">
   <dimension ref="A1:AI117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
seqiential criteria checks added
</commit_message>
<xml_diff>
--- a/Decision Matrices/hierarchy.xlsx
+++ b/Decision Matrices/hierarchy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc3adef44a32c2c0/Documents/GitHub/DP4/Decision Matrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1166" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{783BC90D-2664-4CC3-B68A-4B11ED72BB32}"/>
+  <xr:revisionPtr revIDLastSave="1192" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EB7CAE1-120A-403C-8073-8D012C35D8B8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5770647-7F3F-411D-B267-99FA93025A86}"/>
   </bookViews>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174D7823-B3F8-4046-8216-CB48ECCFAD7A}">
   <dimension ref="A1:AI117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="E38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Importance table completion check
</commit_message>
<xml_diff>
--- a/Decision Matrices/hierarchy.xlsx
+++ b/Decision Matrices/hierarchy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc3adef44a32c2c0/Documents/GitHub/DP4/Decision Matrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1192" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EB7CAE1-120A-403C-8073-8D012C35D8B8}"/>
+  <xr:revisionPtr revIDLastSave="1200" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC589F0E-F580-42B6-A8DF-B9FDDB7185F4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5770647-7F3F-411D-B267-99FA93025A86}"/>
   </bookViews>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174D7823-B3F8-4046-8216-CB48ECCFAD7A}">
   <dimension ref="A1:AI117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Started assembling main. Implemented checks
</commit_message>
<xml_diff>
--- a/Decision Matrices/hierarchy.xlsx
+++ b/Decision Matrices/hierarchy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc3adef44a32c2c0/Documents/GitHub/DP4/Decision Matrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1200" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC589F0E-F580-42B6-A8DF-B9FDDB7185F4}"/>
+  <xr:revisionPtr revIDLastSave="1212" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8538FC0A-998C-4D2E-8CEF-D457DA476625}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5770647-7F3F-411D-B267-99FA93025A86}"/>
   </bookViews>
@@ -134,9 +134,6 @@
     <t>Model Name:</t>
   </si>
   <si>
-    <t>default2</t>
-  </si>
-  <si>
     <t>Random</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>Shoe</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174D7823-B3F8-4046-8216-CB48ECCFAD7A}">
   <dimension ref="A1:AI117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +912,7 @@
       <c r="E2" s="50"/>
       <c r="F2" s="50"/>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H2" s="21" t="s">
         <v>26</v>
@@ -941,16 +941,16 @@
       <c r="F3" s="43"/>
       <c r="G3" s="1"/>
       <c r="H3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="L3" s="10"/>
       <c r="M3" s="13"/>
@@ -1239,7 +1239,7 @@
         <v>20</v>
       </c>
       <c r="H14" s="36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AA14" s="30"/>
       <c r="AB14" s="31"/>
@@ -2363,7 +2363,7 @@
         <v>20</v>
       </c>
       <c r="H35" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA35" s="30"/>
       <c r="AB35" s="31"/>
@@ -3493,7 +3493,7 @@
         <v>20</v>
       </c>
       <c r="H56" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA56" s="30"/>
       <c r="AB56" s="31"/>
@@ -4617,7 +4617,7 @@
         <v>20</v>
       </c>
       <c r="H77" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA77" s="30"/>
       <c r="AB77" s="31"/>

</xml_diff>

<commit_message>
Completed first draft of model creation
</commit_message>
<xml_diff>
--- a/Decision Matrices/hierarchy.xlsx
+++ b/Decision Matrices/hierarchy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc3adef44a32c2c0/Documents/GitHub/DP4/Decision Matrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1212" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8538FC0A-998C-4D2E-8CEF-D457DA476625}"/>
+  <xr:revisionPtr revIDLastSave="1216" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9B75198-E67A-4B42-A0D3-E540FAADC29C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5770647-7F3F-411D-B267-99FA93025A86}"/>
   </bookViews>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174D7823-B3F8-4046-8216-CB48ECCFAD7A}">
   <dimension ref="A1:AI117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Model and log file export
</commit_message>
<xml_diff>
--- a/Decision Matrices/hierarchy.xlsx
+++ b/Decision Matrices/hierarchy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc3adef44a32c2c0/Documents/GitHub/DP4/Decision Matrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1216" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9B75198-E67A-4B42-A0D3-E540FAADC29C}"/>
+  <xr:revisionPtr revIDLastSave="1220" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F723E450-51CE-412A-8235-2C6FB857F335}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5770647-7F3F-411D-B267-99FA93025A86}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5770647-7F3F-411D-B267-99FA93025A86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
patched parent_match check bug
</commit_message>
<xml_diff>
--- a/Decision Matrices/hierarchy.xlsx
+++ b/Decision Matrices/hierarchy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc3adef44a32c2c0/Documents/GitHub/DP4/Decision Matrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1220" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F723E450-51CE-412A-8235-2C6FB857F335}"/>
+  <xr:revisionPtr revIDLastSave="1259" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E070EB6-484D-46D9-9709-9DD212CEA9A8}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5770647-7F3F-411D-B267-99FA93025A86}"/>
   </bookViews>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>Tier 1</t>
-  </si>
-  <si>
-    <t>Drone Type</t>
   </si>
   <si>
     <t>MTOW</t>
@@ -134,19 +131,19 @@
     <t>Model Name:</t>
   </si>
   <si>
-    <t>Random</t>
+    <t>Dimensions</t>
   </si>
   <si>
-    <t>Foo</t>
+    <t>Payload Capibilities</t>
   </si>
   <si>
-    <t>Star</t>
+    <t>Flight Capibilities</t>
   </si>
   <si>
-    <t>Shoe</t>
+    <t>Speed Capibilities</t>
   </si>
   <si>
-    <t>test</t>
+    <t>default_model</t>
   </si>
 </sst>
 </file>
@@ -805,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174D7823-B3F8-4046-8216-CB48ECCFAD7A}">
   <dimension ref="A1:AI117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K81" sqref="K81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,7 +901,7 @@
     </row>
     <row r="2" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -912,22 +909,22 @@
       <c r="E2" s="50"/>
       <c r="F2" s="50"/>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="L2" s="23" t="s">
         <v>29</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -941,18 +938,20 @@
       <c r="F3" s="43"/>
       <c r="G3" s="1"/>
       <c r="H3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>34</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="10"/>
+        <v>31</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -964,7 +963,7 @@
       <c r="F4" s="46"/>
       <c r="G4" s="6" t="str">
         <f>H3</f>
-        <v>Random</v>
+        <v>Flight Capibilities</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -983,58 +982,58 @@
       </c>
       <c r="M4" s="2"/>
       <c r="R4" t="s">
+        <v>14</v>
+      </c>
+      <c r="S4" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" t="s">
         <v>15</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
+        <v>13</v>
+      </c>
+      <c r="V4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF4" t="s">
         <v>3</v>
       </c>
-      <c r="T4" t="s">
-        <v>16</v>
-      </c>
-      <c r="U4" t="s">
-        <v>14</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="AG4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH4" t="s">
         <v>17</v>
       </c>
-      <c r="W4" t="s">
-        <v>9</v>
-      </c>
-      <c r="X4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>7</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG4" t="s">
+      <c r="AI4" t="s">
         <v>5</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1046,7 +1045,7 @@
       <c r="F5" s="46"/>
       <c r="G5" s="7" t="str">
         <f>I3</f>
-        <v>Foo</v>
+        <v>Payload Capibilities</v>
       </c>
       <c r="H5" s="5">
         <f>1/I4</f>
@@ -1126,7 +1125,7 @@
       <c r="F6" s="46"/>
       <c r="G6" s="7" t="str">
         <f>J3</f>
-        <v>Star</v>
+        <v>Speed Capibilities</v>
       </c>
       <c r="H6" s="5">
         <f>1/J4</f>
@@ -1156,7 +1155,7 @@
       <c r="F7" s="46"/>
       <c r="G7" s="7" t="str">
         <f>K3</f>
-        <v>Shoe</v>
+        <v>Dimensions</v>
       </c>
       <c r="H7" s="5">
         <f>1/K4</f>
@@ -1185,9 +1184,9 @@
       <c r="D8" s="48"/>
       <c r="E8" s="48"/>
       <c r="F8" s="49"/>
-      <c r="G8" s="7">
+      <c r="G8" s="7" t="str">
         <f>L3</f>
-        <v>0</v>
+        <v>Drone type</v>
       </c>
       <c r="H8" s="15">
         <f>1/L4</f>
@@ -1228,7 +1227,7 @@
     </row>
     <row r="14" spans="1:35" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
@@ -1236,10 +1235,10 @@
       <c r="E14" s="42"/>
       <c r="F14" s="43"/>
       <c r="G14" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H14" s="36" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AA14" s="30"/>
       <c r="AB14" s="31"/>
@@ -1254,10 +1253,10 @@
       <c r="F15" s="46"/>
       <c r="G15" s="25"/>
       <c r="H15" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="27" t="s">
         <v>7</v>
-      </c>
-      <c r="I15" s="27" t="s">
-        <v>8</v>
       </c>
       <c r="J15" s="27"/>
       <c r="K15" s="27"/>
@@ -2352,7 +2351,7 @@
     </row>
     <row r="35" spans="1:29" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="42"/>
@@ -2360,7 +2359,7 @@
       <c r="E35" s="42"/>
       <c r="F35" s="43"/>
       <c r="G35" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H35" s="36" t="s">
         <v>33</v>
@@ -2378,13 +2377,13 @@
       <c r="F36" s="46"/>
       <c r="G36" s="25"/>
       <c r="H36" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="I36" s="27" t="s">
+      <c r="J36" s="27" t="s">
         <v>10</v>
-      </c>
-      <c r="J36" s="27" t="s">
-        <v>11</v>
       </c>
       <c r="K36" s="27"/>
       <c r="L36" s="27"/>
@@ -3482,7 +3481,7 @@
     </row>
     <row r="56" spans="1:29" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="41" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B56" s="42"/>
       <c r="C56" s="42"/>
@@ -3490,7 +3489,7 @@
       <c r="E56" s="42"/>
       <c r="F56" s="43"/>
       <c r="G56" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H56" s="36" t="s">
         <v>34</v>
@@ -3508,10 +3507,10 @@
       <c r="F57" s="46"/>
       <c r="G57" s="25"/>
       <c r="H57" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I57" s="27" t="s">
         <v>12</v>
-      </c>
-      <c r="I57" s="27" t="s">
-        <v>13</v>
       </c>
       <c r="J57" s="27"/>
       <c r="K57" s="27"/>
@@ -4606,7 +4605,7 @@
     </row>
     <row r="77" spans="1:29" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B77" s="42"/>
       <c r="C77" s="42"/>
@@ -4614,10 +4613,10 @@
       <c r="E77" s="42"/>
       <c r="F77" s="43"/>
       <c r="G77" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H77" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA77" s="30"/>
       <c r="AB77" s="31"/>
@@ -4632,16 +4631,16 @@
       <c r="F78" s="46"/>
       <c r="G78" s="25"/>
       <c r="H78" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I78" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="J78" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="I78" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="J78" s="27" t="s">
-        <v>16</v>
-      </c>
       <c r="K78" s="27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L78" s="27"/>
       <c r="M78" s="27"/>
@@ -5744,7 +5743,7 @@
     </row>
     <row r="98" spans="1:29" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B98" s="42"/>
       <c r="C98" s="42"/>
@@ -5752,10 +5751,10 @@
       <c r="E98" s="42"/>
       <c r="F98" s="43"/>
       <c r="G98" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H98" s="36" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AA98" s="30"/>
       <c r="AB98" s="31"/>
@@ -5770,16 +5769,16 @@
       <c r="F99" s="46"/>
       <c r="G99" s="25"/>
       <c r="H99" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="I99" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="I99" s="27" t="s">
+      <c r="J99" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="K99" s="27" t="s">
         <v>5</v>
-      </c>
-      <c r="J99" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="K99" s="27" t="s">
-        <v>6</v>
       </c>
       <c r="L99" s="27"/>
       <c r="M99" s="27"/>
@@ -5815,13 +5814,13 @@
         <v>1</v>
       </c>
       <c r="I100" s="39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J100" s="39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K100" s="39">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L100" s="39"/>
       <c r="M100" s="39"/>
@@ -5855,16 +5854,16 @@
       </c>
       <c r="H101" s="40">
         <f>1/I100</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I101" s="39">
         <v>1</v>
       </c>
       <c r="J101" s="39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K101" s="39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L101" s="39"/>
       <c r="M101" s="39"/>
@@ -5898,17 +5897,17 @@
       </c>
       <c r="H102" s="40">
         <f>1/J100</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I102" s="39">
         <f>1/J101</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J102" s="39">
         <v>1</v>
       </c>
       <c r="K102" s="39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L102" s="39"/>
       <c r="M102" s="39"/>
@@ -5942,15 +5941,15 @@
       </c>
       <c r="H103" s="40">
         <f>1/K100</f>
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="I103" s="40">
         <f>1/K101</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J103" s="40">
         <f>1/K102</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K103" s="39">
         <v>1</v>

</xml_diff>

<commit_message>
Fixed TypeError when calculating eigenvalues
</commit_message>
<xml_diff>
--- a/Decision Matrices/hierarchy.xlsx
+++ b/Decision Matrices/hierarchy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc3adef44a32c2c0/Documents/GitHub/DP4/Decision Matrices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1268" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8217A190-717D-4E67-986E-C67E35CDBE54}"/>
+  <xr:revisionPtr revIDLastSave="1269" documentId="8_{463FBA96-44C3-4641-8427-C26223F7EA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBFA6A42-A403-4D99-93C0-81A47CA99B8D}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5770647-7F3F-411D-B267-99FA93025A86}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5770647-7F3F-411D-B267-99FA93025A86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
     <t>Speed Capibilities</t>
   </si>
   <si>
-    <t>default2</t>
+    <t>eigentest</t>
   </si>
 </sst>
 </file>
@@ -503,6 +503,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -792,7 +796,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -802,30 +806,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174D7823-B3F8-4046-8216-CB48ECCFAD7A}">
   <dimension ref="A1:AI117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="62" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.90625" customWidth="1"/>
-    <col min="7" max="7" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="25" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.1796875" customWidth="1"/>
-    <col min="33" max="33" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="25" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.21875" customWidth="1"/>
+    <col min="33" max="33" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>0</v>
       </c>
@@ -899,7 +903,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="50" t="s">
         <v>30</v>
       </c>
@@ -927,7 +931,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="41" t="s">
         <v>0</v>
       </c>
@@ -954,7 +958,7 @@
       </c>
       <c r="M3" s="13"/>
     </row>
-    <row r="4" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="44"/>
       <c r="B4" s="45"/>
       <c r="C4" s="45"/>
@@ -1036,7 +1040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="44"/>
       <c r="B5" s="45"/>
       <c r="C5" s="45"/>
@@ -1116,7 +1120,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="44"/>
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
@@ -1146,7 +1150,7 @@
       </c>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="44"/>
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
@@ -1177,7 +1181,7 @@
       </c>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:35" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:35" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="47"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
@@ -1208,24 +1212,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:35" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
     </row>
-    <row r="10" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
     </row>
-    <row r="11" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
     </row>
-    <row r="12" spans="1:35" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:35" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18"/>
     </row>
-    <row r="13" spans="1:35" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:35" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AA13" s="34"/>
       <c r="AB13" s="35"/>
       <c r="AC13" s="35"/>
     </row>
-    <row r="14" spans="1:35" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:35" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="41" t="s">
         <v>20</v>
       </c>
@@ -1244,7 +1248,7 @@
       <c r="AB14" s="31"/>
       <c r="AC14" s="32"/>
     </row>
-    <row r="15" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="44"/>
       <c r="B15" s="45"/>
       <c r="C15" s="45"/>
@@ -1279,7 +1283,7 @@
       <c r="AB15" s="3"/>
       <c r="AC15" s="4"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" s="44"/>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
@@ -1317,7 +1321,7 @@
       <c r="AB16" s="3"/>
       <c r="AC16" s="20"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="44"/>
       <c r="B17" s="45"/>
       <c r="C17" s="45"/>
@@ -1356,7 +1360,7 @@
       <c r="AB17" s="3"/>
       <c r="AC17" s="4"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="44"/>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
@@ -1398,7 +1402,7 @@
       <c r="AB18" s="3"/>
       <c r="AC18" s="20"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="44"/>
       <c r="B19" s="45"/>
       <c r="C19" s="45"/>
@@ -1443,7 +1447,7 @@
       <c r="AB19" s="3"/>
       <c r="AC19" s="4"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="44"/>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
@@ -1491,7 +1495,7 @@
       <c r="AB20" s="3"/>
       <c r="AC20" s="20"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="44"/>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
@@ -1542,7 +1546,7 @@
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="44"/>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -1596,7 +1600,7 @@
       <c r="AB22" s="20"/>
       <c r="AC22" s="20"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="44"/>
       <c r="B23" s="45"/>
       <c r="C23" s="45"/>
@@ -1649,7 +1653,7 @@
       <c r="X23" s="39"/>
       <c r="Y23" s="39"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="44"/>
       <c r="B24" s="45"/>
       <c r="C24" s="45"/>
@@ -1705,7 +1709,7 @@
       <c r="X24" s="39"/>
       <c r="Y24" s="39"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="44"/>
       <c r="B25" s="45"/>
       <c r="C25" s="45"/>
@@ -1764,7 +1768,7 @@
       <c r="X25" s="39"/>
       <c r="Y25" s="39"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="44"/>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
@@ -1826,7 +1830,7 @@
       <c r="X26" s="39"/>
       <c r="Y26" s="39"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="44"/>
       <c r="B27" s="45"/>
       <c r="C27" s="45"/>
@@ -1891,7 +1895,7 @@
       <c r="X27" s="39"/>
       <c r="Y27" s="39"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="44"/>
       <c r="B28" s="45"/>
       <c r="C28" s="45"/>
@@ -1959,7 +1963,7 @@
       <c r="X28" s="39"/>
       <c r="Y28" s="39"/>
     </row>
-    <row r="29" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="44"/>
       <c r="B29" s="45"/>
       <c r="C29" s="45"/>
@@ -2030,7 +2034,7 @@
       <c r="X29" s="39"/>
       <c r="Y29" s="39"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="44"/>
       <c r="B30" s="45"/>
       <c r="C30" s="45"/>
@@ -2104,7 +2108,7 @@
       <c r="X30" s="39"/>
       <c r="Y30" s="39"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="44"/>
       <c r="B31" s="45"/>
       <c r="C31" s="45"/>
@@ -2181,7 +2185,7 @@
       <c r="X31" s="39"/>
       <c r="Y31" s="39"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="44"/>
       <c r="B32" s="45"/>
       <c r="C32" s="45"/>
@@ -2261,7 +2265,7 @@
       </c>
       <c r="Y32" s="39"/>
     </row>
-    <row r="33" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="47"/>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
@@ -2344,12 +2348,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:29" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:29" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AA34" s="34"/>
       <c r="AB34" s="35"/>
       <c r="AC34" s="35"/>
     </row>
-    <row r="35" spans="1:29" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:29" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="41" t="s">
         <v>21</v>
       </c>
@@ -2368,7 +2372,7 @@
       <c r="AB35" s="31"/>
       <c r="AC35" s="32"/>
     </row>
-    <row r="36" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="44"/>
       <c r="B36" s="45"/>
       <c r="C36" s="45"/>
@@ -2405,7 +2409,7 @@
       <c r="AB36" s="3"/>
       <c r="AC36" s="4"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" s="44"/>
       <c r="B37" s="45"/>
       <c r="C37" s="45"/>
@@ -2445,7 +2449,7 @@
       <c r="AB37" s="3"/>
       <c r="AC37" s="20"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" s="44"/>
       <c r="B38" s="45"/>
       <c r="C38" s="45"/>
@@ -2486,7 +2490,7 @@
       <c r="AB38" s="3"/>
       <c r="AC38" s="4"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="44"/>
       <c r="B39" s="45"/>
       <c r="C39" s="45"/>
@@ -2528,7 +2532,7 @@
       <c r="AB39" s="3"/>
       <c r="AC39" s="20"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="44"/>
       <c r="B40" s="45"/>
       <c r="C40" s="45"/>
@@ -2573,7 +2577,7 @@
       <c r="AB40" s="3"/>
       <c r="AC40" s="4"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="44"/>
       <c r="B41" s="45"/>
       <c r="C41" s="45"/>
@@ -2621,7 +2625,7 @@
       <c r="AB41" s="3"/>
       <c r="AC41" s="20"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42" s="44"/>
       <c r="B42" s="45"/>
       <c r="C42" s="45"/>
@@ -2672,7 +2676,7 @@
       <c r="AB42" s="4"/>
       <c r="AC42" s="4"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" s="44"/>
       <c r="B43" s="45"/>
       <c r="C43" s="45"/>
@@ -2726,7 +2730,7 @@
       <c r="AB43" s="20"/>
       <c r="AC43" s="20"/>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44" s="44"/>
       <c r="B44" s="45"/>
       <c r="C44" s="45"/>
@@ -2779,7 +2783,7 @@
       <c r="X44" s="39"/>
       <c r="Y44" s="39"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" s="44"/>
       <c r="B45" s="45"/>
       <c r="C45" s="45"/>
@@ -2835,7 +2839,7 @@
       <c r="X45" s="39"/>
       <c r="Y45" s="39"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" s="44"/>
       <c r="B46" s="45"/>
       <c r="C46" s="45"/>
@@ -2894,7 +2898,7 @@
       <c r="X46" s="39"/>
       <c r="Y46" s="39"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" s="44"/>
       <c r="B47" s="45"/>
       <c r="C47" s="45"/>
@@ -2956,7 +2960,7 @@
       <c r="X47" s="39"/>
       <c r="Y47" s="39"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48" s="44"/>
       <c r="B48" s="45"/>
       <c r="C48" s="45"/>
@@ -3021,7 +3025,7 @@
       <c r="X48" s="39"/>
       <c r="Y48" s="39"/>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49" s="44"/>
       <c r="B49" s="45"/>
       <c r="C49" s="45"/>
@@ -3089,7 +3093,7 @@
       <c r="X49" s="39"/>
       <c r="Y49" s="39"/>
     </row>
-    <row r="50" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="44"/>
       <c r="B50" s="45"/>
       <c r="C50" s="45"/>
@@ -3160,7 +3164,7 @@
       <c r="X50" s="39"/>
       <c r="Y50" s="39"/>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51" s="44"/>
       <c r="B51" s="45"/>
       <c r="C51" s="45"/>
@@ -3234,7 +3238,7 @@
       <c r="X51" s="39"/>
       <c r="Y51" s="39"/>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A52" s="44"/>
       <c r="B52" s="45"/>
       <c r="C52" s="45"/>
@@ -3311,7 +3315,7 @@
       <c r="X52" s="39"/>
       <c r="Y52" s="39"/>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A53" s="44"/>
       <c r="B53" s="45"/>
       <c r="C53" s="45"/>
@@ -3391,7 +3395,7 @@
       </c>
       <c r="Y53" s="39"/>
     </row>
-    <row r="54" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="47"/>
       <c r="B54" s="48"/>
       <c r="C54" s="48"/>
@@ -3474,12 +3478,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:29" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:29" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AA55" s="34"/>
       <c r="AB55" s="35"/>
       <c r="AC55" s="35"/>
     </row>
-    <row r="56" spans="1:29" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:29" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="41" t="s">
         <v>22</v>
       </c>
@@ -3498,7 +3502,7 @@
       <c r="AB56" s="31"/>
       <c r="AC56" s="32"/>
     </row>
-    <row r="57" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="44"/>
       <c r="B57" s="45"/>
       <c r="C57" s="45"/>
@@ -3533,7 +3537,7 @@
       <c r="AB57" s="3"/>
       <c r="AC57" s="4"/>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A58" s="44"/>
       <c r="B58" s="45"/>
       <c r="C58" s="45"/>
@@ -3571,7 +3575,7 @@
       <c r="AB58" s="3"/>
       <c r="AC58" s="20"/>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A59" s="44"/>
       <c r="B59" s="45"/>
       <c r="C59" s="45"/>
@@ -3610,7 +3614,7 @@
       <c r="AB59" s="3"/>
       <c r="AC59" s="4"/>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A60" s="44"/>
       <c r="B60" s="45"/>
       <c r="C60" s="45"/>
@@ -3652,7 +3656,7 @@
       <c r="AB60" s="3"/>
       <c r="AC60" s="20"/>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A61" s="44"/>
       <c r="B61" s="45"/>
       <c r="C61" s="45"/>
@@ -3697,7 +3701,7 @@
       <c r="AB61" s="3"/>
       <c r="AC61" s="4"/>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A62" s="44"/>
       <c r="B62" s="45"/>
       <c r="C62" s="45"/>
@@ -3745,7 +3749,7 @@
       <c r="AB62" s="3"/>
       <c r="AC62" s="20"/>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A63" s="44"/>
       <c r="B63" s="45"/>
       <c r="C63" s="45"/>
@@ -3796,7 +3800,7 @@
       <c r="AB63" s="4"/>
       <c r="AC63" s="4"/>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" s="44"/>
       <c r="B64" s="45"/>
       <c r="C64" s="45"/>
@@ -3850,7 +3854,7 @@
       <c r="AB64" s="20"/>
       <c r="AC64" s="20"/>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65" s="44"/>
       <c r="B65" s="45"/>
       <c r="C65" s="45"/>
@@ -3903,7 +3907,7 @@
       <c r="X65" s="39"/>
       <c r="Y65" s="39"/>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A66" s="44"/>
       <c r="B66" s="45"/>
       <c r="C66" s="45"/>
@@ -3959,7 +3963,7 @@
       <c r="X66" s="39"/>
       <c r="Y66" s="39"/>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A67" s="44"/>
       <c r="B67" s="45"/>
       <c r="C67" s="45"/>
@@ -4018,7 +4022,7 @@
       <c r="X67" s="39"/>
       <c r="Y67" s="39"/>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A68" s="44"/>
       <c r="B68" s="45"/>
       <c r="C68" s="45"/>
@@ -4080,7 +4084,7 @@
       <c r="X68" s="39"/>
       <c r="Y68" s="39"/>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A69" s="44"/>
       <c r="B69" s="45"/>
       <c r="C69" s="45"/>
@@ -4145,7 +4149,7 @@
       <c r="X69" s="39"/>
       <c r="Y69" s="39"/>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A70" s="44"/>
       <c r="B70" s="45"/>
       <c r="C70" s="45"/>
@@ -4213,7 +4217,7 @@
       <c r="X70" s="39"/>
       <c r="Y70" s="39"/>
     </row>
-    <row r="71" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="44"/>
       <c r="B71" s="45"/>
       <c r="C71" s="45"/>
@@ -4284,7 +4288,7 @@
       <c r="X71" s="39"/>
       <c r="Y71" s="39"/>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72" s="44"/>
       <c r="B72" s="45"/>
       <c r="C72" s="45"/>
@@ -4358,7 +4362,7 @@
       <c r="X72" s="39"/>
       <c r="Y72" s="39"/>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73" s="44"/>
       <c r="B73" s="45"/>
       <c r="C73" s="45"/>
@@ -4435,7 +4439,7 @@
       <c r="X73" s="39"/>
       <c r="Y73" s="39"/>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A74" s="44"/>
       <c r="B74" s="45"/>
       <c r="C74" s="45"/>
@@ -4515,7 +4519,7 @@
       </c>
       <c r="Y74" s="39"/>
     </row>
-    <row r="75" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="47"/>
       <c r="B75" s="48"/>
       <c r="C75" s="48"/>
@@ -4598,12 +4602,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:29" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:29" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AA76" s="34"/>
       <c r="AB76" s="35"/>
       <c r="AC76" s="35"/>
     </row>
-    <row r="77" spans="1:29" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:29" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="41" t="s">
         <v>23</v>
       </c>
@@ -4622,7 +4626,7 @@
       <c r="AB77" s="31"/>
       <c r="AC77" s="32"/>
     </row>
-    <row r="78" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="44"/>
       <c r="B78" s="45"/>
       <c r="C78" s="45"/>
@@ -4661,7 +4665,7 @@
       <c r="AB78" s="3"/>
       <c r="AC78" s="4"/>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79" s="44"/>
       <c r="B79" s="45"/>
       <c r="C79" s="45"/>
@@ -4703,7 +4707,7 @@
       <c r="AB79" s="3"/>
       <c r="AC79" s="20"/>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A80" s="44"/>
       <c r="B80" s="45"/>
       <c r="C80" s="45"/>
@@ -4746,7 +4750,7 @@
       <c r="AB80" s="3"/>
       <c r="AC80" s="4"/>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A81" s="44"/>
       <c r="B81" s="45"/>
       <c r="C81" s="45"/>
@@ -4790,7 +4794,7 @@
       <c r="AB81" s="3"/>
       <c r="AC81" s="20"/>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A82" s="44"/>
       <c r="B82" s="45"/>
       <c r="C82" s="45"/>
@@ -4835,7 +4839,7 @@
       <c r="AB82" s="3"/>
       <c r="AC82" s="4"/>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A83" s="44"/>
       <c r="B83" s="45"/>
       <c r="C83" s="45"/>
@@ -4883,7 +4887,7 @@
       <c r="AB83" s="3"/>
       <c r="AC83" s="20"/>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A84" s="44"/>
       <c r="B84" s="45"/>
       <c r="C84" s="45"/>
@@ -4934,7 +4938,7 @@
       <c r="AB84" s="4"/>
       <c r="AC84" s="4"/>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A85" s="44"/>
       <c r="B85" s="45"/>
       <c r="C85" s="45"/>
@@ -4988,7 +4992,7 @@
       <c r="AB85" s="20"/>
       <c r="AC85" s="20"/>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A86" s="44"/>
       <c r="B86" s="45"/>
       <c r="C86" s="45"/>
@@ -5041,7 +5045,7 @@
       <c r="X86" s="39"/>
       <c r="Y86" s="39"/>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A87" s="44"/>
       <c r="B87" s="45"/>
       <c r="C87" s="45"/>
@@ -5097,7 +5101,7 @@
       <c r="X87" s="39"/>
       <c r="Y87" s="39"/>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A88" s="44"/>
       <c r="B88" s="45"/>
       <c r="C88" s="45"/>
@@ -5156,7 +5160,7 @@
       <c r="X88" s="39"/>
       <c r="Y88" s="39"/>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A89" s="44"/>
       <c r="B89" s="45"/>
       <c r="C89" s="45"/>
@@ -5218,7 +5222,7 @@
       <c r="X89" s="39"/>
       <c r="Y89" s="39"/>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A90" s="44"/>
       <c r="B90" s="45"/>
       <c r="C90" s="45"/>
@@ -5283,7 +5287,7 @@
       <c r="X90" s="39"/>
       <c r="Y90" s="39"/>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A91" s="44"/>
       <c r="B91" s="45"/>
       <c r="C91" s="45"/>
@@ -5351,7 +5355,7 @@
       <c r="X91" s="39"/>
       <c r="Y91" s="39"/>
     </row>
-    <row r="92" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="44"/>
       <c r="B92" s="45"/>
       <c r="C92" s="45"/>
@@ -5422,7 +5426,7 @@
       <c r="X92" s="39"/>
       <c r="Y92" s="39"/>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A93" s="44"/>
       <c r="B93" s="45"/>
       <c r="C93" s="45"/>
@@ -5496,7 +5500,7 @@
       <c r="X93" s="39"/>
       <c r="Y93" s="39"/>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A94" s="44"/>
       <c r="B94" s="45"/>
       <c r="C94" s="45"/>
@@ -5573,7 +5577,7 @@
       <c r="X94" s="39"/>
       <c r="Y94" s="39"/>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A95" s="44"/>
       <c r="B95" s="45"/>
       <c r="C95" s="45"/>
@@ -5653,7 +5657,7 @@
       </c>
       <c r="Y95" s="39"/>
     </row>
-    <row r="96" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="47"/>
       <c r="B96" s="48"/>
       <c r="C96" s="48"/>
@@ -5736,12 +5740,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:29" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:29" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AA97" s="34"/>
       <c r="AB97" s="35"/>
       <c r="AC97" s="35"/>
     </row>
-    <row r="98" spans="1:29" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:29" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="41" t="s">
         <v>24</v>
       </c>
@@ -5760,7 +5764,7 @@
       <c r="AB98" s="31"/>
       <c r="AC98" s="32"/>
     </row>
-    <row r="99" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="44"/>
       <c r="B99" s="45"/>
       <c r="C99" s="45"/>
@@ -5799,7 +5803,7 @@
       <c r="AB99" s="3"/>
       <c r="AC99" s="4"/>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A100" s="44"/>
       <c r="B100" s="45"/>
       <c r="C100" s="45"/>
@@ -5841,7 +5845,7 @@
       <c r="AB100" s="3"/>
       <c r="AC100" s="20"/>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A101" s="44"/>
       <c r="B101" s="45"/>
       <c r="C101" s="45"/>
@@ -5884,7 +5888,7 @@
       <c r="AB101" s="3"/>
       <c r="AC101" s="4"/>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A102" s="44"/>
       <c r="B102" s="45"/>
       <c r="C102" s="45"/>
@@ -5928,7 +5932,7 @@
       <c r="AB102" s="3"/>
       <c r="AC102" s="20"/>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A103" s="44"/>
       <c r="B103" s="45"/>
       <c r="C103" s="45"/>
@@ -5973,7 +5977,7 @@
       <c r="AB103" s="3"/>
       <c r="AC103" s="4"/>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A104" s="44"/>
       <c r="B104" s="45"/>
       <c r="C104" s="45"/>
@@ -6021,7 +6025,7 @@
       <c r="AB104" s="3"/>
       <c r="AC104" s="20"/>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A105" s="44"/>
       <c r="B105" s="45"/>
       <c r="C105" s="45"/>
@@ -6072,7 +6076,7 @@
       <c r="AB105" s="4"/>
       <c r="AC105" s="4"/>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A106" s="44"/>
       <c r="B106" s="45"/>
       <c r="C106" s="45"/>
@@ -6126,7 +6130,7 @@
       <c r="AB106" s="20"/>
       <c r="AC106" s="20"/>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A107" s="44"/>
       <c r="B107" s="45"/>
       <c r="C107" s="45"/>
@@ -6179,7 +6183,7 @@
       <c r="X107" s="39"/>
       <c r="Y107" s="39"/>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A108" s="44"/>
       <c r="B108" s="45"/>
       <c r="C108" s="45"/>
@@ -6235,7 +6239,7 @@
       <c r="X108" s="39"/>
       <c r="Y108" s="39"/>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A109" s="44"/>
       <c r="B109" s="45"/>
       <c r="C109" s="45"/>
@@ -6294,7 +6298,7 @@
       <c r="X109" s="39"/>
       <c r="Y109" s="39"/>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A110" s="44"/>
       <c r="B110" s="45"/>
       <c r="C110" s="45"/>
@@ -6356,7 +6360,7 @@
       <c r="X110" s="39"/>
       <c r="Y110" s="39"/>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A111" s="44"/>
       <c r="B111" s="45"/>
       <c r="C111" s="45"/>
@@ -6421,7 +6425,7 @@
       <c r="X111" s="39"/>
       <c r="Y111" s="39"/>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A112" s="44"/>
       <c r="B112" s="45"/>
       <c r="C112" s="45"/>
@@ -6489,7 +6493,7 @@
       <c r="X112" s="39"/>
       <c r="Y112" s="39"/>
     </row>
-    <row r="113" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="44"/>
       <c r="B113" s="45"/>
       <c r="C113" s="45"/>
@@ -6560,7 +6564,7 @@
       <c r="X113" s="39"/>
       <c r="Y113" s="39"/>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A114" s="44"/>
       <c r="B114" s="45"/>
       <c r="C114" s="45"/>
@@ -6634,7 +6638,7 @@
       <c r="X114" s="39"/>
       <c r="Y114" s="39"/>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A115" s="44"/>
       <c r="B115" s="45"/>
       <c r="C115" s="45"/>
@@ -6711,7 +6715,7 @@
       <c r="X115" s="39"/>
       <c r="Y115" s="39"/>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A116" s="44"/>
       <c r="B116" s="45"/>
       <c r="C116" s="45"/>
@@ -6791,7 +6795,7 @@
       </c>
       <c r="Y116" s="39"/>
     </row>
-    <row r="117" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="47"/>
       <c r="B117" s="48"/>
       <c r="C117" s="48"/>

</xml_diff>